<commit_message>
Send Invoice/ Payment receipt to customer #CRM-403
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
+++ b/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>{meta:company_name}</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">Invoice Date: {meta:invoice_date}								</t>
-  </si>
-  <si>
-    <t>Invoice Date: {meta:invoice_date}</t>
   </si>
   <si>
     <t>Reverse Charge (Y/N):</t>
@@ -192,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="42">
     <border/>
     <border>
       <left style="thin">
@@ -465,21 +462,6 @@
       <top/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -510,15 +492,6 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -556,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -605,11 +578,10 @@
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,21 +597,21 @@
     <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="26" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="28" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -654,9 +626,6 @@
     <xf borderId="7" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="36" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -669,32 +638,31 @@
     <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="35" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="37" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="38" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="39" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="41" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="42" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="43" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="38" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="39" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="44" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="45" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="41" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,464 +862,448 @@
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-    </row>
-    <row r="9">
+      <c r="J8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="27"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29"/>
+    </row>
+    <row r="9" ht="10.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="27" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="19"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" ht="10.5" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="19"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="33"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="34"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="25"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="5"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="29"/>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="30"/>
-    </row>
-    <row r="15">
+      <c r="B14" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="41"/>
+    </row>
+    <row r="15" ht="10.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="41" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="42"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="S15" s="42"/>
-    </row>
-    <row r="16" ht="10.5" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="43"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="45"/>
+      <c r="L16" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="45"/>
+      <c r="N16" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="46"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" s="16"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="46"/>
-      <c r="L17" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="47"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="48" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="19"/>
+    </row>
+    <row r="18" ht="28.5" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="R17" s="16"/>
-      <c r="S17" s="17"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="25"/>
+      <c r="N18" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="51" t="s">
+        <v>24</v>
+      </c>
       <c r="R18" s="14"/>
       <c r="S18" s="19"/>
     </row>
-    <row r="19" ht="28.5" customHeight="1">
+    <row r="19" ht="6.0" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="25"/>
-      <c r="L19" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" s="25"/>
-      <c r="N19" s="53" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="52"/>
+    </row>
+    <row r="20" ht="30.0" customHeight="1">
+      <c r="A20" s="1"/>
+      <c r="B20" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="19"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="24"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="R19" s="14"/>
-      <c r="S19" s="19"/>
-    </row>
-    <row r="20" ht="6.0" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="56"/>
-    </row>
-    <row r="21" ht="30.0" customHeight="1">
+      <c r="R20" s="14"/>
+      <c r="S20" s="19"/>
+    </row>
+    <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="61" t="s">
+      <c r="B21" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="R21" s="14"/>
-      <c r="S21" s="19"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="62"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="59"/>
     </row>
     <row r="23">
       <c r="A23" s="1"/>
-      <c r="B23" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="64"/>
+      <c r="B23" s="11"/>
+      <c r="S23" s="60"/>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="11"/>
-      <c r="S24" s="65"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="42"/>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="43"/>
+      <c r="B25" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="1"/>
-      <c r="B26" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="G26" s="10"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="29"/>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="11"/>
       <c r="G27" s="10"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="30"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="11"/>
       <c r="G28" s="10"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="5"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="11"/>
+      <c r="S28" s="10"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="11"/>
       <c r="G29" s="10"/>
-      <c r="J29" s="65"/>
+      <c r="J29" s="60"/>
       <c r="K29" s="11"/>
       <c r="S29" s="10"/>
     </row>
@@ -1359,123 +1311,113 @@
       <c r="A30" s="1"/>
       <c r="B30" s="11"/>
       <c r="G30" s="10"/>
-      <c r="J30" s="65"/>
+      <c r="J30" s="60"/>
       <c r="K30" s="11"/>
       <c r="S30" s="10"/>
     </row>
-    <row r="31">
+    <row r="31" ht="0.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="11"/>
       <c r="G31" s="10"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="11"/>
-      <c r="S31" s="10"/>
-    </row>
-    <row r="32" ht="0.75" customHeight="1">
+      <c r="J31" s="60"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="29"/>
+    </row>
+    <row r="32">
       <c r="A32" s="1"/>
-      <c r="B32" s="11"/>
-      <c r="G32" s="10"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="30"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="29"/>
     </row>
     <row r="33">
       <c r="A33" s="1"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="69" t="s">
-        <v>32</v>
-      </c>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="29"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="30"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="B23:S25"/>
-    <mergeCell ref="J17:K18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:S20"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="B16:S16"/>
-    <mergeCell ref="B22:S22"/>
-    <mergeCell ref="K9:S9"/>
+  <mergeCells count="42">
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="B5:S6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B15:S15"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="B12:S13"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="B16:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:S19"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L16:M17"/>
+    <mergeCell ref="K25:S26"/>
+    <mergeCell ref="K27:S31"/>
+    <mergeCell ref="B25:G32"/>
+    <mergeCell ref="K32:S32"/>
+    <mergeCell ref="H25:J32"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="B22:S24"/>
+    <mergeCell ref="B21:S21"/>
+    <mergeCell ref="B11:S11"/>
     <mergeCell ref="B10:S10"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="F3:Q3"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="K7:S7"/>
+    <mergeCell ref="K8:S8"/>
+    <mergeCell ref="B9:S9"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="N16:P17"/>
+    <mergeCell ref="Q16:S17"/>
     <mergeCell ref="B7:J7"/>
-    <mergeCell ref="K8:S8"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="B13:S14"/>
-    <mergeCell ref="B12:S12"/>
-    <mergeCell ref="B11:S11"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B5:S6"/>
-    <mergeCell ref="K7:S7"/>
-    <mergeCell ref="K26:S27"/>
-    <mergeCell ref="K28:S32"/>
-    <mergeCell ref="B26:G33"/>
-    <mergeCell ref="K33:S33"/>
-    <mergeCell ref="H26:J33"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q17:S18"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="J15:Q15"/>
-    <mergeCell ref="B17:I18"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="N17:P18"/>
-    <mergeCell ref="L17:M18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add booking id in Customer Invoice and Change Customer sms #CRM-446
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
+++ b/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>{meta:company_name}</t>
   </si>
@@ -31,13 +31,16 @@
     <t>Invoice No: {meta:invoice_id}</t>
   </si>
   <si>
+    <t xml:space="preserve">Booking ID: {meta:booking_id}                                                                </t>
+  </si>
+  <si>
+    <t>Reverse Charge (Y/N):</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Invoice Date: {meta:invoice_date}								</t>
-  </si>
-  <si>
-    <t>Reverse Charge (Y/N):</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Bill to Party</t>
@@ -317,12 +320,18 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -330,7 +339,10 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -341,15 +353,20 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -357,20 +374,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -529,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -578,39 +581,42 @@
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="20" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="20" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="23" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="24" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="26" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="28" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -626,16 +632,16 @@
     <xf borderId="7" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -649,6 +655,9 @@
     </xf>
     <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -865,19 +874,21 @@
       <c r="J8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="29"/>
+      <c r="K8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="25"/>
     </row>
     <row r="9" ht="10.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="30"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -898,31 +909,31 @@
     </row>
     <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="33"/>
+      <c r="B10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="34" t="s">
-        <v>10</v>
+      <c r="B11" s="32" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -944,8 +955,8 @@
     </row>
     <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="35" t="s">
-        <v>11</v>
+      <c r="B12" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -967,55 +978,55 @@
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="29"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38" t="s">
+      <c r="B14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="40" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="S14" s="41"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" s="42"/>
     </row>
     <row r="15" ht="10.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="30"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1032,12 +1043,12 @@
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
-      <c r="S15" s="42"/>
+      <c r="S15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="43" t="s">
-        <v>15</v>
+      <c r="B16" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1046,21 +1057,21 @@
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="45"/>
-      <c r="L16" s="44" t="s">
+      <c r="J16" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="45"/>
-      <c r="N16" s="44" t="s">
+      <c r="K16" s="46"/>
+      <c r="L16" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="O16" s="46"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="47" t="s">
+      <c r="M16" s="46"/>
+      <c r="N16" s="45" t="s">
         <v>19</v>
+      </c>
+      <c r="O16" s="47"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="48" t="s">
+        <v>20</v>
       </c>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
@@ -1087,8 +1098,8 @@
     </row>
     <row r="18" ht="28.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="48" t="s">
-        <v>20</v>
+      <c r="B18" s="49" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -1097,21 +1108,21 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="49" t="s">
-        <v>21</v>
+      <c r="J18" s="50" t="s">
+        <v>22</v>
       </c>
       <c r="K18" s="25"/>
-      <c r="L18" s="50" t="s">
-        <v>22</v>
+      <c r="L18" s="51" t="s">
+        <v>23</v>
       </c>
       <c r="M18" s="25"/>
-      <c r="N18" s="49" t="s">
-        <v>23</v>
+      <c r="N18" s="50" t="s">
+        <v>24</v>
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="25"/>
-      <c r="Q18" s="51" t="s">
-        <v>24</v>
+      <c r="Q18" s="52" t="s">
+        <v>25</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="19"/>
@@ -1135,62 +1146,62 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
-      <c r="S19" s="52"/>
+      <c r="S19" s="53"/>
     </row>
     <row r="20" ht="30.0" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
+      <c r="B20" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="57" t="s">
-        <v>26</v>
+      <c r="L20" s="58" t="s">
+        <v>27</v>
       </c>
       <c r="M20" s="19"/>
-      <c r="N20" s="51"/>
+      <c r="N20" s="59"/>
       <c r="O20" s="14"/>
       <c r="P20" s="19"/>
-      <c r="Q20" s="51" t="s">
-        <v>24</v>
+      <c r="Q20" s="59" t="s">
+        <v>25</v>
       </c>
       <c r="R20" s="14"/>
       <c r="S20" s="19"/>
     </row>
     <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
+      <c r="B21" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="58" t="s">
-        <v>28</v>
+      <c r="B22" s="60" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -1208,12 +1219,12 @@
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
-      <c r="S22" s="59"/>
+      <c r="S22" s="61"/>
     </row>
     <row r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="11"/>
-      <c r="S23" s="60"/>
+      <c r="S23" s="62"/>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
@@ -1234,23 +1245,23 @@
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
-      <c r="S24" s="42"/>
+      <c r="S24" s="43"/>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="61" t="s">
-        <v>29</v>
+      <c r="B25" s="63" t="s">
+        <v>30</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="62"/>
+      <c r="H25" s="64"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="61" t="s">
-        <v>30</v>
+      <c r="J25" s="61"/>
+      <c r="K25" s="63" t="s">
+        <v>31</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1265,23 +1276,23 @@
       <c r="A26" s="1"/>
       <c r="B26" s="11"/>
       <c r="G26" s="10"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="29"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="36"/>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="11"/>
       <c r="G27" s="10"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="61"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1295,7 +1306,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="11"/>
       <c r="G28" s="10"/>
-      <c r="J28" s="60"/>
+      <c r="J28" s="62"/>
       <c r="K28" s="11"/>
       <c r="S28" s="10"/>
     </row>
@@ -1303,7 +1314,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="11"/>
       <c r="G29" s="10"/>
-      <c r="J29" s="60"/>
+      <c r="J29" s="62"/>
       <c r="K29" s="11"/>
       <c r="S29" s="10"/>
     </row>
@@ -1311,7 +1322,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="11"/>
       <c r="G30" s="10"/>
-      <c r="J30" s="60"/>
+      <c r="J30" s="62"/>
       <c r="K30" s="11"/>
       <c r="S30" s="10"/>
     </row>
@@ -1319,39 +1330,39 @@
       <c r="A31" s="1"/>
       <c r="B31" s="11"/>
       <c r="G31" s="10"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="29"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="36"/>
     </row>
     <row r="32">
       <c r="A32" s="1"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="28"/>
-      <c r="S32" s="29"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="36"/>
     </row>
     <row r="33">
       <c r="A33" s="1"/>
@@ -1377,47 +1388,47 @@
   </sheetData>
   <mergeCells count="42">
     <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="B11:S11"/>
+    <mergeCell ref="B10:S10"/>
+    <mergeCell ref="B9:S9"/>
     <mergeCell ref="B5:S6"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="F3:Q3"/>
     <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B15:S15"/>
-    <mergeCell ref="J14:Q14"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="R3:S4"/>
     <mergeCell ref="B12:S13"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="H20:K20"/>
     <mergeCell ref="J16:K17"/>
     <mergeCell ref="B16:I17"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:S19"/>
+    <mergeCell ref="N20:P20"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L16:M17"/>
+    <mergeCell ref="Q16:S17"/>
+    <mergeCell ref="B15:S15"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="B19:S19"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="B2:S2"/>
     <mergeCell ref="K25:S26"/>
+    <mergeCell ref="B22:S24"/>
     <mergeCell ref="K27:S31"/>
     <mergeCell ref="B25:G32"/>
     <mergeCell ref="K32:S32"/>
     <mergeCell ref="H25:J32"/>
-    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="B20:G20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="B22:S24"/>
     <mergeCell ref="B21:S21"/>
-    <mergeCell ref="B11:S11"/>
-    <mergeCell ref="B10:S10"/>
     <mergeCell ref="K7:S7"/>
     <mergeCell ref="K8:S8"/>
-    <mergeCell ref="B9:S9"/>
-    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="L16:M17"/>
     <mergeCell ref="N16:P17"/>
-    <mergeCell ref="Q16:S17"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
#CRM-727 Add 247Around Logo in Customer Invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
+++ b/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED32DA7-80F9-4690-9848-F714BD988A6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
@@ -124,8 +125,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -687,76 +688,87 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -777,6 +789,25 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -784,36 +815,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,6 +830,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB5465B-8C6A-4D28-B9A8-D62138F9C0CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142874" y="123824"/>
+          <a:ext cx="695325" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1127,34 +1183,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="0.83203125" customWidth="1"/>
-    <col min="2" max="2" width="2.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="0.5" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="10" width="4.6640625" customWidth="1"/>
-    <col min="11" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" customWidth="1"/>
-    <col min="13" max="13" width="3.5" customWidth="1"/>
-    <col min="14" max="14" width="4.5" customWidth="1"/>
-    <col min="15" max="15" width="1.6640625" customWidth="1"/>
-    <col min="16" max="16" width="3.83203125" customWidth="1"/>
-    <col min="17" max="17" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="0.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" customWidth="1"/>
+    <col min="15" max="15" width="1.7109375" customWidth="1"/>
+    <col min="16" max="16" width="3.85546875" customWidth="1"/>
+    <col min="17" max="17" width="3.28515625" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" customWidth="1"/>
-    <col min="20" max="26" width="12.5" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" customWidth="1"/>
+    <col min="20" max="26" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="3.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1175,726 +1233,726 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="28"/>
-    </row>
-    <row r="3" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8" t="s">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="9"/>
-    </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="S3" s="22"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75">
       <c r="A4" s="1"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="9"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="43"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="18"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="41"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1"/>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="67" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="13"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="27"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1"/>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
       <c r="J8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="67" t="s">
+      <c r="K8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="13"/>
-    </row>
-    <row r="9" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="27"/>
+    </row>
+    <row r="9" spans="1:19" ht="10.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="18"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="48"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="41"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1"/>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="16"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="62"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="13"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1"/>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="28"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="31"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1"/>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="47" t="s">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="44" t="s">
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="S14" s="45"/>
-    </row>
-    <row r="15" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="52"/>
+    </row>
+    <row r="15" spans="1:19" ht="10.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="41"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="48"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="33" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="34"/>
-      <c r="L16" s="33" t="s">
+      <c r="K16" s="37"/>
+      <c r="L16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="N16" s="33" t="s">
+      <c r="M16" s="37"/>
+      <c r="N16" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="68"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="40" t="s">
+      <c r="O16" s="38"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="20"/>
-      <c r="S16" s="21"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R16" s="14"/>
+      <c r="S16" s="43"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="18"/>
-    </row>
-    <row r="18" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="41"/>
+    </row>
+    <row r="18" spans="1:19" ht="50.1" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="38" t="s">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="63" t="s">
+      <c r="K18" s="27"/>
+      <c r="L18" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="13"/>
-      <c r="N18" s="38" t="s">
+      <c r="M18" s="27"/>
+      <c r="N18" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="39" t="s">
+      <c r="O18" s="35"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="7"/>
-      <c r="S18" s="18"/>
-    </row>
-    <row r="19" spans="1:19" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R18" s="20"/>
+      <c r="S18" s="41"/>
+    </row>
+    <row r="19" spans="1:19" ht="6" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="51"/>
-    </row>
-    <row r="20" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="58"/>
+    </row>
+    <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="46" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="37" t="s">
+      <c r="M20" s="41"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="R20" s="7"/>
-      <c r="S20" s="18"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R20" s="20"/>
+      <c r="S20" s="41"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1"/>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1"/>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="58"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="15"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="59"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="18"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="41"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1"/>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="56" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="28"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="31"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="12"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="28"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="9"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="22"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="9"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="22"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="9"/>
-    </row>
-    <row r="31" spans="1:19" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="22"/>
+    </row>
+    <row r="31" spans="1:19" ht="0.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="31"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="12"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="60" t="s">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="31"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="12"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1917,6 +1975,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="B19:S19"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="B11:S11"/>
+    <mergeCell ref="B10:S10"/>
+    <mergeCell ref="B9:S9"/>
+    <mergeCell ref="B5:S6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q16:S17"/>
+    <mergeCell ref="B15:S15"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="B16:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="L20:M20"/>
     <mergeCell ref="B2:S2"/>
     <mergeCell ref="K25:S26"/>
     <mergeCell ref="B22:S24"/>
@@ -1933,33 +2017,8 @@
     <mergeCell ref="L16:M17"/>
     <mergeCell ref="N16:P17"/>
     <mergeCell ref="B12:S13"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="J16:K17"/>
-    <mergeCell ref="B16:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q16:S17"/>
-    <mergeCell ref="B15:S15"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="J14:Q14"/>
-    <mergeCell ref="B19:S19"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="B11:S11"/>
-    <mergeCell ref="B10:S10"/>
-    <mergeCell ref="B9:S9"/>
-    <mergeCell ref="B5:S6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="F3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify code for main partner invoicing detail
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
+++ b/application/controllers/excel-templates/Customer_FOC_Bill_of_Supply.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC868611-CFE7-4D14-ACF8-F82620EDC484}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169CF204-9E7D-4D65-A19A-4FB92D518296}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:S33"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>